<commit_message>
fixed data error for vote share for candidate 1 in Ha Noi district 1
</commit_message>
<xml_diff>
--- a/Data/Results/Result_2016.xlsx
+++ b/Data/Results/Result_2016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5495,23 +5495,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5547,23 +5530,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5719,7 +5685,7 @@
   <dimension ref="A1:I871"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5784,7 +5750,7 @@
         <v>299827</v>
       </c>
       <c r="H2">
-        <v>86.47</v>
+        <v>72.67</v>
       </c>
       <c r="I2">
         <v>1</v>

</xml_diff>